<commit_message>
feat: auto-change on seat summary
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/Books-mix.xlsx
+++ b/spec/fixtures/files/Books-mix.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">VVIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
   </si>
   <si>
     <t xml:space="preserve">test13</t>
@@ -450,7 +453,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -545,10 +548,10 @@
         <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>3.3</v>
@@ -556,13 +559,13 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>19</v>
@@ -579,13 +582,13 @@
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>10</v>

</xml_diff>